<commit_message>
adição no banco de dados
</commit_message>
<xml_diff>
--- a/dataBases/dataBase-cpu.xlsx
+++ b/dataBases/dataBase-cpu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f7782c7c2999047/Documentos/Facul/Away/Repositórios/Combinação de Hardware/dataBases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_AC644A91FE4F4DF7E942289308C2A6458A66E95C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53A8C5D-2664-4D59-ABB7-78631D27A84C}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_AC644A91FE4F4DF7E942289308C2A6458A66E95C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D88D0F-F189-4F82-9ED8-02642F42F3B2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Game</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>ryzen 3 3200G</t>
+  </si>
+  <si>
+    <t>367.4</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,6 +526,17 @@
         <v>289</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>